<commit_message>
change some classification of comments
</commit_message>
<xml_diff>
--- a/public/討論區留言.xlsx
+++ b/public/討論區留言.xlsx
@@ -1770,7 +1770,7 @@
     <t>HEHEMan</t>
   </si>
   <si>
-    <t>對生命的愛護是很好的，但是要執行也要有好的解決方案，不是說只有改條例而已，能提出方案內容才是更改法令最好的條件，而不是一股腦的附譯</t>
+    <t>友善航班是很好，但是要執行也要有好的配套措施，而不是一股腦地開放</t>
   </si>
   <si>
     <t>2024-06-17 17:40:44</t>
@@ -2481,7 +2481,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2500,6 +2500,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3056,7 +3065,7 @@
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -3080,14 +3089,14 @@
       <c r="J7" s="6">
         <v>0.0</v>
       </c>
-      <c r="K7" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0.0</v>
+      <c r="K7" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1.0</v>
       </c>
       <c r="N7" s="6">
         <v>0.0</v>
@@ -3238,28 +3247,28 @@
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="11">
         <v>92.0</v>
       </c>
-      <c r="G11" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>57</v>
       </c>
       <c r="I11" s="6">
@@ -3283,16 +3292,16 @@
       <c r="O11" s="6">
         <v>0.0</v>
       </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -3930,8 +3939,8 @@
       <c r="H25" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I25" s="6">
-        <v>1.0</v>
+      <c r="I25" s="10">
+        <v>0.0</v>
       </c>
       <c r="J25" s="6">
         <v>0.0</v>
@@ -3939,14 +3948,14 @@
       <c r="K25" s="6">
         <v>0.0</v>
       </c>
-      <c r="L25" s="6">
-        <v>1.0</v>
+      <c r="L25" s="10">
+        <v>0.0</v>
       </c>
       <c r="M25" s="6">
         <v>0.0</v>
       </c>
-      <c r="N25" s="6">
-        <v>1.0</v>
+      <c r="N25" s="10">
+        <v>0.0</v>
       </c>
       <c r="O25" s="6">
         <v>0.0</v>
@@ -4000,28 +4009,28 @@
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="11">
         <v>55.0</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="11">
         <v>2.0</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="12" t="s">
         <v>121</v>
       </c>
       <c r="I27" s="6">
@@ -4045,16 +4054,16 @@
       <c r="O27" s="6">
         <v>0.0</v>
       </c>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -5068,11 +5077,11 @@
       <c r="H49" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I49" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="J49" s="6">
-        <v>0.0</v>
+      <c r="I49" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="J49" s="10">
+        <v>1.0</v>
       </c>
       <c r="K49" s="6">
         <v>0.0</v>
@@ -5232,28 +5241,28 @@
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="11">
         <v>2.0</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="11">
         <v>4.0</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H53" s="12" t="s">
         <v>226</v>
       </c>
       <c r="I53" s="6">
@@ -5271,22 +5280,22 @@
       <c r="M53" s="6">
         <v>0.0</v>
       </c>
-      <c r="N53" s="12">
+      <c r="N53" s="15">
         <v>1.0</v>
       </c>
       <c r="O53" s="6">
         <v>0.0</v>
       </c>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
-      <c r="V53" s="11"/>
-      <c r="W53" s="11"/>
-      <c r="X53" s="11"/>
-      <c r="Y53" s="11"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="14"/>
+      <c r="X53" s="14"/>
+      <c r="Y53" s="14"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="2" t="s">
@@ -5524,28 +5533,28 @@
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F59" s="11">
         <v>4.0</v>
       </c>
-      <c r="G59" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H59" s="9" t="s">
+      <c r="G59" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H59" s="12" t="s">
         <v>249</v>
       </c>
       <c r="I59" s="6">
@@ -5569,16 +5578,16 @@
       <c r="O59" s="6">
         <v>0.0</v>
       </c>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
-      <c r="T59" s="11"/>
-      <c r="U59" s="11"/>
-      <c r="V59" s="11"/>
-      <c r="W59" s="11"/>
-      <c r="X59" s="11"/>
-      <c r="Y59" s="11"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="14"/>
+      <c r="V59" s="14"/>
+      <c r="W59" s="14"/>
+      <c r="X59" s="14"/>
+      <c r="Y59" s="14"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="2" t="s">
@@ -5634,7 +5643,7 @@
       <c r="B61" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="8" t="s">
         <v>256</v>
       </c>
       <c r="D61" s="5" t="s">
@@ -5722,28 +5731,28 @@
       </c>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F63" s="11">
         <v>5.0</v>
       </c>
-      <c r="G63" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H63" s="9" t="s">
+      <c r="G63" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H63" s="12" t="s">
         <v>264</v>
       </c>
       <c r="I63" s="6">
@@ -5767,40 +5776,40 @@
       <c r="O63" s="6">
         <v>0.0</v>
       </c>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
-      <c r="T63" s="11"/>
-      <c r="U63" s="11"/>
-      <c r="V63" s="11"/>
-      <c r="W63" s="11"/>
-      <c r="X63" s="11"/>
-      <c r="Y63" s="11"/>
+      <c r="P63" s="14"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="14"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="14"/>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="14"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F64" s="8">
+      <c r="F64" s="11">
         <v>6.0</v>
       </c>
-      <c r="G64" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H64" s="9" t="s">
+      <c r="G64" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H64" s="12" t="s">
         <v>268</v>
       </c>
       <c r="I64" s="6">
@@ -5824,16 +5833,16 @@
       <c r="O64" s="6">
         <v>0.0</v>
       </c>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11"/>
-      <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="11"/>
-      <c r="W64" s="11"/>
-      <c r="X64" s="11"/>
-      <c r="Y64" s="11"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="14"/>
+      <c r="V64" s="14"/>
+      <c r="W64" s="14"/>
+      <c r="X64" s="14"/>
+      <c r="Y64" s="14"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="2" t="s">
@@ -5977,13 +5986,13 @@
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="17" t="s">
         <v>283</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -5992,10 +6001,10 @@
       <c r="E68" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="13">
+      <c r="F68" s="16">
         <v>3.0</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="16">
         <v>4.0</v>
       </c>
       <c r="H68" s="5" t="s">
@@ -6010,7 +6019,7 @@
       <c r="K68" s="6">
         <v>0.0</v>
       </c>
-      <c r="L68" s="15">
+      <c r="L68" s="18">
         <v>1.0</v>
       </c>
       <c r="M68" s="6">
@@ -6022,14 +6031,14 @@
       <c r="O68" s="6">
         <v>0.0</v>
       </c>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="18"/>
+      <c r="U68" s="18"/>
+      <c r="V68" s="18"/>
+      <c r="W68" s="18"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="2" t="s">
@@ -6455,13 +6464,13 @@
       </c>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="20" t="s">
         <v>324</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -6470,10 +6479,10 @@
       <c r="E78" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F78" s="16">
+      <c r="F78" s="19">
         <v>3.0</v>
       </c>
-      <c r="G78" s="16">
+      <c r="G78" s="19">
         <v>2.0</v>
       </c>
       <c r="H78" s="5" t="s">
@@ -6491,7 +6500,7 @@
       <c r="L78" s="6">
         <v>0.0</v>
       </c>
-      <c r="M78" s="18">
+      <c r="M78" s="21">
         <v>1.0</v>
       </c>
       <c r="N78" s="6">
@@ -6500,38 +6509,38 @@
       <c r="O78" s="6">
         <v>0.0</v>
       </c>
-      <c r="P78" s="18"/>
-      <c r="Q78" s="18"/>
-      <c r="R78" s="18"/>
-      <c r="S78" s="18"/>
-      <c r="T78" s="18"/>
-      <c r="U78" s="18"/>
-      <c r="V78" s="18"/>
-      <c r="W78" s="18"/>
+      <c r="P78" s="21"/>
+      <c r="Q78" s="21"/>
+      <c r="R78" s="21"/>
+      <c r="S78" s="21"/>
+      <c r="T78" s="21"/>
+      <c r="U78" s="21"/>
+      <c r="V78" s="21"/>
+      <c r="W78" s="21"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C79" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="E79" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F79" s="8">
+      <c r="F79" s="11">
         <v>4.0</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79" s="11">
         <v>2.0</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="H79" s="12" t="s">
         <v>329</v>
       </c>
       <c r="I79" s="6">
@@ -6555,16 +6564,16 @@
       <c r="O79" s="6">
         <v>0.0</v>
       </c>
-      <c r="P79" s="11"/>
-      <c r="Q79" s="11"/>
-      <c r="R79" s="11"/>
-      <c r="S79" s="11"/>
-      <c r="T79" s="11"/>
-      <c r="U79" s="11"/>
-      <c r="V79" s="11"/>
-      <c r="W79" s="11"/>
-      <c r="X79" s="11"/>
-      <c r="Y79" s="11"/>
+      <c r="P79" s="14"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="14"/>
+      <c r="S79" s="14"/>
+      <c r="T79" s="14"/>
+      <c r="U79" s="14"/>
+      <c r="V79" s="14"/>
+      <c r="W79" s="14"/>
+      <c r="X79" s="14"/>
+      <c r="Y79" s="14"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="2" t="s">
@@ -6708,28 +6717,28 @@
       </c>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D83" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F83" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="G83" s="8">
+      <c r="F83" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="G83" s="11">
         <v>3.0</v>
       </c>
-      <c r="H83" s="9" t="s">
+      <c r="H83" s="12" t="s">
         <v>345</v>
       </c>
       <c r="I83" s="6">
@@ -6753,16 +6762,16 @@
       <c r="O83" s="6">
         <v>0.0</v>
       </c>
-      <c r="P83" s="11"/>
-      <c r="Q83" s="11"/>
-      <c r="R83" s="11"/>
-      <c r="S83" s="11"/>
-      <c r="T83" s="11"/>
-      <c r="U83" s="11"/>
-      <c r="V83" s="11"/>
-      <c r="W83" s="11"/>
-      <c r="X83" s="11"/>
-      <c r="Y83" s="11"/>
+      <c r="P83" s="14"/>
+      <c r="Q83" s="14"/>
+      <c r="R83" s="14"/>
+      <c r="S83" s="14"/>
+      <c r="T83" s="14"/>
+      <c r="U83" s="14"/>
+      <c r="V83" s="14"/>
+      <c r="W83" s="14"/>
+      <c r="X83" s="14"/>
+      <c r="Y83" s="14"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="2" t="s">
@@ -6859,13 +6868,13 @@
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="23" t="s">
         <v>356</v>
       </c>
       <c r="D86" s="5" t="s">
@@ -6874,10 +6883,10 @@
       <c r="E86" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F86" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="G86" s="19">
+      <c r="F86" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="G86" s="22">
         <v>0.0</v>
       </c>
       <c r="H86" s="5" t="s">
@@ -6904,14 +6913,14 @@
       <c r="O86" s="6">
         <v>0.0</v>
       </c>
-      <c r="P86" s="21"/>
-      <c r="Q86" s="21"/>
-      <c r="R86" s="21"/>
-      <c r="S86" s="21"/>
-      <c r="T86" s="21"/>
-      <c r="U86" s="21"/>
-      <c r="V86" s="21"/>
-      <c r="W86" s="21"/>
+      <c r="P86" s="24"/>
+      <c r="Q86" s="24"/>
+      <c r="R86" s="24"/>
+      <c r="S86" s="24"/>
+      <c r="T86" s="24"/>
+      <c r="U86" s="24"/>
+      <c r="V86" s="24"/>
+      <c r="W86" s="24"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="2" t="s">
@@ -6961,28 +6970,28 @@
       </c>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C88" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="D88" s="9" t="s">
+      <c r="D88" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="E88" s="10" t="s">
+      <c r="E88" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F88" s="8">
+      <c r="F88" s="11">
         <v>3.0</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88" s="11">
         <v>2.0</v>
       </c>
-      <c r="H88" s="9" t="s">
+      <c r="H88" s="12" t="s">
         <v>366</v>
       </c>
       <c r="I88" s="6">
@@ -7006,40 +7015,40 @@
       <c r="O88" s="6">
         <v>0.0</v>
       </c>
-      <c r="P88" s="11"/>
-      <c r="Q88" s="11"/>
-      <c r="R88" s="11"/>
-      <c r="S88" s="11"/>
-      <c r="T88" s="11"/>
-      <c r="U88" s="11"/>
-      <c r="V88" s="11"/>
-      <c r="W88" s="11"/>
-      <c r="X88" s="11"/>
-      <c r="Y88" s="11"/>
+      <c r="P88" s="14"/>
+      <c r="Q88" s="14"/>
+      <c r="R88" s="14"/>
+      <c r="S88" s="14"/>
+      <c r="T88" s="14"/>
+      <c r="U88" s="14"/>
+      <c r="V88" s="14"/>
+      <c r="W88" s="14"/>
+      <c r="X88" s="14"/>
+      <c r="Y88" s="14"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D89" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="E89" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F89" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G89" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H89" s="9" t="s">
+      <c r="F89" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="G89" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H89" s="12" t="s">
         <v>370</v>
       </c>
       <c r="I89" s="6">
@@ -7063,40 +7072,40 @@
       <c r="O89" s="6">
         <v>0.0</v>
       </c>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="11"/>
-      <c r="W89" s="11"/>
-      <c r="X89" s="11"/>
-      <c r="Y89" s="11"/>
+      <c r="P89" s="14"/>
+      <c r="Q89" s="14"/>
+      <c r="R89" s="14"/>
+      <c r="S89" s="14"/>
+      <c r="T89" s="14"/>
+      <c r="U89" s="14"/>
+      <c r="V89" s="14"/>
+      <c r="W89" s="14"/>
+      <c r="X89" s="14"/>
+      <c r="Y89" s="14"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="D90" s="9" t="s">
+      <c r="D90" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E90" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F90" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G90" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H90" s="9" t="s">
+      <c r="F90" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="G90" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H90" s="12" t="s">
         <v>374</v>
       </c>
       <c r="I90" s="6">
@@ -7120,40 +7129,40 @@
       <c r="O90" s="6">
         <v>0.0</v>
       </c>
-      <c r="P90" s="11"/>
-      <c r="Q90" s="11"/>
-      <c r="R90" s="11"/>
-      <c r="S90" s="11"/>
-      <c r="T90" s="11"/>
-      <c r="U90" s="11"/>
-      <c r="V90" s="11"/>
-      <c r="W90" s="11"/>
-      <c r="X90" s="11"/>
-      <c r="Y90" s="11"/>
+      <c r="P90" s="14"/>
+      <c r="Q90" s="14"/>
+      <c r="R90" s="14"/>
+      <c r="S90" s="14"/>
+      <c r="T90" s="14"/>
+      <c r="U90" s="14"/>
+      <c r="V90" s="14"/>
+      <c r="W90" s="14"/>
+      <c r="X90" s="14"/>
+      <c r="Y90" s="14"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C91" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="D91" s="9" t="s">
+      <c r="D91" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F91" s="8">
+      <c r="F91" s="11">
         <v>3.0</v>
       </c>
-      <c r="G91" s="8">
+      <c r="G91" s="11">
         <v>2.0</v>
       </c>
-      <c r="H91" s="9" t="s">
+      <c r="H91" s="12" t="s">
         <v>378</v>
       </c>
       <c r="I91" s="6">
@@ -7177,616 +7186,616 @@
       <c r="O91" s="6">
         <v>0.0</v>
       </c>
-      <c r="P91" s="11"/>
-      <c r="Q91" s="11"/>
-      <c r="R91" s="11"/>
-      <c r="S91" s="11"/>
-      <c r="T91" s="11"/>
-      <c r="U91" s="11"/>
-      <c r="V91" s="11"/>
-      <c r="W91" s="11"/>
-      <c r="X91" s="11"/>
-      <c r="Y91" s="11"/>
+      <c r="P91" s="14"/>
+      <c r="Q91" s="14"/>
+      <c r="R91" s="14"/>
+      <c r="S91" s="14"/>
+      <c r="T91" s="14"/>
+      <c r="U91" s="14"/>
+      <c r="V91" s="14"/>
+      <c r="W91" s="14"/>
+      <c r="X91" s="14"/>
+      <c r="Y91" s="14"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="C92" s="22"/>
+      <c r="C92" s="25"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="C93" s="22"/>
+      <c r="C93" s="25"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="C94" s="22"/>
+      <c r="C94" s="25"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="C95" s="22"/>
+      <c r="C95" s="25"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="C96" s="22"/>
+      <c r="C96" s="25"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="C97" s="22"/>
+      <c r="C97" s="25"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="C98" s="22"/>
+      <c r="C98" s="25"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="C99" s="22"/>
+      <c r="C99" s="25"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="C100" s="22"/>
+      <c r="C100" s="25"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="C101" s="22"/>
+      <c r="C101" s="25"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="C102" s="22"/>
+      <c r="C102" s="25"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="C103" s="22"/>
+      <c r="C103" s="25"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="C104" s="22"/>
+      <c r="C104" s="25"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="C105" s="22"/>
+      <c r="C105" s="25"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="C106" s="22"/>
+      <c r="C106" s="25"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="C107" s="22"/>
+      <c r="C107" s="25"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="C108" s="22"/>
+      <c r="C108" s="25"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="C109" s="22"/>
+      <c r="C109" s="25"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="C110" s="22"/>
+      <c r="C110" s="25"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="C111" s="22"/>
+      <c r="C111" s="25"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="C112" s="22"/>
+      <c r="C112" s="25"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="C113" s="22"/>
+      <c r="C113" s="25"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="C114" s="22"/>
+      <c r="C114" s="25"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="C115" s="22"/>
+      <c r="C115" s="25"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="C116" s="22"/>
+      <c r="C116" s="25"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="C117" s="22"/>
+      <c r="C117" s="25"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="C118" s="22"/>
+      <c r="C118" s="25"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="C119" s="22"/>
+      <c r="C119" s="25"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="C120" s="22"/>
+      <c r="C120" s="25"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="C121" s="22"/>
+      <c r="C121" s="25"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="C122" s="22"/>
+      <c r="C122" s="25"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
-      <c r="C123" s="22"/>
+      <c r="C123" s="25"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="C124" s="22"/>
+      <c r="C124" s="25"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="C125" s="22"/>
+      <c r="C125" s="25"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="C126" s="22"/>
+      <c r="C126" s="25"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="C127" s="22"/>
+      <c r="C127" s="25"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="C128" s="22"/>
+      <c r="C128" s="25"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="C129" s="22"/>
+      <c r="C129" s="25"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
-      <c r="C130" s="22"/>
+      <c r="C130" s="25"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
-      <c r="C131" s="22"/>
+      <c r="C131" s="25"/>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="C132" s="22"/>
+      <c r="C132" s="25"/>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="C133" s="22"/>
+      <c r="C133" s="25"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="C134" s="22"/>
+      <c r="C134" s="25"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="C135" s="22"/>
+      <c r="C135" s="25"/>
     </row>
     <row r="136" ht="12.75" customHeight="1">
-      <c r="C136" s="22"/>
+      <c r="C136" s="25"/>
     </row>
     <row r="137" ht="12.75" customHeight="1">
-      <c r="C137" s="22"/>
+      <c r="C137" s="25"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
-      <c r="C138" s="22"/>
+      <c r="C138" s="25"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
-      <c r="C139" s="22"/>
+      <c r="C139" s="25"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
-      <c r="C140" s="22"/>
+      <c r="C140" s="25"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="C141" s="22"/>
+      <c r="C141" s="25"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
-      <c r="C142" s="22"/>
+      <c r="C142" s="25"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
-      <c r="C143" s="22"/>
+      <c r="C143" s="25"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
-      <c r="C144" s="22"/>
+      <c r="C144" s="25"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
-      <c r="C145" s="22"/>
+      <c r="C145" s="25"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
-      <c r="C146" s="22"/>
+      <c r="C146" s="25"/>
     </row>
     <row r="147" ht="12.75" customHeight="1">
-      <c r="C147" s="22"/>
+      <c r="C147" s="25"/>
     </row>
     <row r="148" ht="12.75" customHeight="1">
-      <c r="C148" s="22"/>
+      <c r="C148" s="25"/>
     </row>
     <row r="149" ht="12.75" customHeight="1">
-      <c r="C149" s="22"/>
+      <c r="C149" s="25"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
-      <c r="C150" s="22"/>
+      <c r="C150" s="25"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
-      <c r="C151" s="22"/>
+      <c r="C151" s="25"/>
     </row>
     <row r="152" ht="12.75" customHeight="1">
-      <c r="C152" s="22"/>
+      <c r="C152" s="25"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
-      <c r="C153" s="22"/>
+      <c r="C153" s="25"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="C154" s="22"/>
+      <c r="C154" s="25"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
-      <c r="C155" s="22"/>
+      <c r="C155" s="25"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
-      <c r="C156" s="22"/>
+      <c r="C156" s="25"/>
     </row>
     <row r="157" ht="12.75" customHeight="1">
-      <c r="C157" s="22"/>
+      <c r="C157" s="25"/>
     </row>
     <row r="158" ht="12.75" customHeight="1">
-      <c r="C158" s="22"/>
+      <c r="C158" s="25"/>
     </row>
     <row r="159" ht="12.75" customHeight="1">
-      <c r="C159" s="22"/>
+      <c r="C159" s="25"/>
     </row>
     <row r="160" ht="12.75" customHeight="1">
-      <c r="C160" s="22"/>
+      <c r="C160" s="25"/>
     </row>
     <row r="161" ht="12.75" customHeight="1">
-      <c r="C161" s="22"/>
+      <c r="C161" s="25"/>
     </row>
     <row r="162" ht="12.75" customHeight="1">
-      <c r="C162" s="22"/>
+      <c r="C162" s="25"/>
     </row>
     <row r="163" ht="12.75" customHeight="1">
-      <c r="C163" s="22"/>
+      <c r="C163" s="25"/>
     </row>
     <row r="164" ht="12.75" customHeight="1">
-      <c r="C164" s="22"/>
+      <c r="C164" s="25"/>
     </row>
     <row r="165" ht="12.75" customHeight="1">
-      <c r="C165" s="22"/>
+      <c r="C165" s="25"/>
     </row>
     <row r="166" ht="12.75" customHeight="1">
-      <c r="C166" s="22"/>
+      <c r="C166" s="25"/>
     </row>
     <row r="167" ht="12.75" customHeight="1">
-      <c r="C167" s="22"/>
+      <c r="C167" s="25"/>
     </row>
     <row r="168" ht="12.75" customHeight="1">
-      <c r="C168" s="22"/>
+      <c r="C168" s="25"/>
     </row>
     <row r="169" ht="12.75" customHeight="1">
-      <c r="C169" s="22"/>
+      <c r="C169" s="25"/>
     </row>
     <row r="170" ht="12.75" customHeight="1">
-      <c r="C170" s="22"/>
+      <c r="C170" s="25"/>
     </row>
     <row r="171" ht="12.75" customHeight="1">
-      <c r="C171" s="22"/>
+      <c r="C171" s="25"/>
     </row>
     <row r="172" ht="12.75" customHeight="1">
-      <c r="C172" s="22"/>
+      <c r="C172" s="25"/>
     </row>
     <row r="173" ht="12.75" customHeight="1">
-      <c r="C173" s="22"/>
+      <c r="C173" s="25"/>
     </row>
     <row r="174" ht="12.75" customHeight="1">
-      <c r="C174" s="22"/>
+      <c r="C174" s="25"/>
     </row>
     <row r="175" ht="12.75" customHeight="1">
-      <c r="C175" s="22"/>
+      <c r="C175" s="25"/>
     </row>
     <row r="176" ht="12.75" customHeight="1">
-      <c r="C176" s="22"/>
+      <c r="C176" s="25"/>
     </row>
     <row r="177" ht="12.75" customHeight="1">
-      <c r="C177" s="22"/>
+      <c r="C177" s="25"/>
     </row>
     <row r="178" ht="12.75" customHeight="1">
-      <c r="C178" s="22"/>
+      <c r="C178" s="25"/>
     </row>
     <row r="179" ht="12.75" customHeight="1">
-      <c r="C179" s="22"/>
+      <c r="C179" s="25"/>
     </row>
     <row r="180" ht="12.75" customHeight="1">
-      <c r="C180" s="22"/>
+      <c r="C180" s="25"/>
     </row>
     <row r="181" ht="12.75" customHeight="1">
-      <c r="C181" s="22"/>
+      <c r="C181" s="25"/>
     </row>
     <row r="182" ht="12.75" customHeight="1">
-      <c r="C182" s="22"/>
+      <c r="C182" s="25"/>
     </row>
     <row r="183" ht="12.75" customHeight="1">
-      <c r="C183" s="22"/>
+      <c r="C183" s="25"/>
     </row>
     <row r="184" ht="12.75" customHeight="1">
-      <c r="C184" s="22"/>
+      <c r="C184" s="25"/>
     </row>
     <row r="185" ht="12.75" customHeight="1">
-      <c r="C185" s="22"/>
+      <c r="C185" s="25"/>
     </row>
     <row r="186" ht="12.75" customHeight="1">
-      <c r="C186" s="22"/>
+      <c r="C186" s="25"/>
     </row>
     <row r="187" ht="12.75" customHeight="1">
-      <c r="C187" s="22"/>
+      <c r="C187" s="25"/>
     </row>
     <row r="188" ht="12.75" customHeight="1">
-      <c r="C188" s="22"/>
+      <c r="C188" s="25"/>
     </row>
     <row r="189" ht="12.75" customHeight="1">
-      <c r="C189" s="22"/>
+      <c r="C189" s="25"/>
     </row>
     <row r="190" ht="12.75" customHeight="1">
-      <c r="C190" s="22"/>
+      <c r="C190" s="25"/>
     </row>
     <row r="191" ht="12.75" customHeight="1">
-      <c r="C191" s="22"/>
+      <c r="C191" s="25"/>
     </row>
     <row r="192" ht="12.75" customHeight="1">
-      <c r="C192" s="22"/>
+      <c r="C192" s="25"/>
     </row>
     <row r="193" ht="12.75" customHeight="1">
-      <c r="C193" s="22"/>
+      <c r="C193" s="25"/>
     </row>
     <row r="194" ht="12.75" customHeight="1">
-      <c r="C194" s="22"/>
+      <c r="C194" s="25"/>
     </row>
     <row r="195" ht="12.75" customHeight="1">
-      <c r="C195" s="22"/>
+      <c r="C195" s="25"/>
     </row>
     <row r="196" ht="12.75" customHeight="1">
-      <c r="C196" s="22"/>
+      <c r="C196" s="25"/>
     </row>
     <row r="197" ht="12.75" customHeight="1">
-      <c r="C197" s="22"/>
+      <c r="C197" s="25"/>
     </row>
     <row r="198" ht="12.75" customHeight="1">
-      <c r="C198" s="22"/>
+      <c r="C198" s="25"/>
     </row>
     <row r="199" ht="12.75" customHeight="1">
-      <c r="C199" s="22"/>
+      <c r="C199" s="25"/>
     </row>
     <row r="200" ht="12.75" customHeight="1">
-      <c r="C200" s="22"/>
+      <c r="C200" s="25"/>
     </row>
     <row r="201" ht="12.75" customHeight="1">
-      <c r="C201" s="22"/>
+      <c r="C201" s="25"/>
     </row>
     <row r="202" ht="12.75" customHeight="1">
-      <c r="C202" s="22"/>
+      <c r="C202" s="25"/>
     </row>
     <row r="203" ht="12.75" customHeight="1">
-      <c r="C203" s="22"/>
+      <c r="C203" s="25"/>
     </row>
     <row r="204" ht="12.75" customHeight="1">
-      <c r="C204" s="22"/>
+      <c r="C204" s="25"/>
     </row>
     <row r="205" ht="12.75" customHeight="1">
-      <c r="C205" s="22"/>
+      <c r="C205" s="25"/>
     </row>
     <row r="206" ht="12.75" customHeight="1">
-      <c r="C206" s="22"/>
+      <c r="C206" s="25"/>
     </row>
     <row r="207" ht="12.75" customHeight="1">
-      <c r="C207" s="22"/>
+      <c r="C207" s="25"/>
     </row>
     <row r="208" ht="12.75" customHeight="1">
-      <c r="C208" s="22"/>
+      <c r="C208" s="25"/>
     </row>
     <row r="209" ht="12.75" customHeight="1">
-      <c r="C209" s="22"/>
+      <c r="C209" s="25"/>
     </row>
     <row r="210" ht="12.75" customHeight="1">
-      <c r="C210" s="22"/>
+      <c r="C210" s="25"/>
     </row>
     <row r="211" ht="12.75" customHeight="1">
-      <c r="C211" s="22"/>
+      <c r="C211" s="25"/>
     </row>
     <row r="212" ht="12.75" customHeight="1">
-      <c r="C212" s="22"/>
+      <c r="C212" s="25"/>
     </row>
     <row r="213" ht="12.75" customHeight="1">
-      <c r="C213" s="22"/>
+      <c r="C213" s="25"/>
     </row>
     <row r="214" ht="12.75" customHeight="1">
-      <c r="C214" s="22"/>
+      <c r="C214" s="25"/>
     </row>
     <row r="215" ht="12.75" customHeight="1">
-      <c r="C215" s="22"/>
+      <c r="C215" s="25"/>
     </row>
     <row r="216" ht="12.75" customHeight="1">
-      <c r="C216" s="22"/>
+      <c r="C216" s="25"/>
     </row>
     <row r="217" ht="12.75" customHeight="1">
-      <c r="C217" s="22"/>
+      <c r="C217" s="25"/>
     </row>
     <row r="218" ht="12.75" customHeight="1">
-      <c r="C218" s="22"/>
+      <c r="C218" s="25"/>
     </row>
     <row r="219" ht="12.75" customHeight="1">
-      <c r="C219" s="22"/>
+      <c r="C219" s="25"/>
     </row>
     <row r="220" ht="12.75" customHeight="1">
-      <c r="C220" s="22"/>
+      <c r="C220" s="25"/>
     </row>
     <row r="221" ht="12.75" customHeight="1">
-      <c r="C221" s="22"/>
+      <c r="C221" s="25"/>
     </row>
     <row r="222" ht="12.75" customHeight="1">
-      <c r="C222" s="22"/>
+      <c r="C222" s="25"/>
     </row>
     <row r="223" ht="12.75" customHeight="1">
-      <c r="C223" s="22"/>
+      <c r="C223" s="25"/>
     </row>
     <row r="224" ht="12.75" customHeight="1">
-      <c r="C224" s="22"/>
+      <c r="C224" s="25"/>
     </row>
     <row r="225" ht="12.75" customHeight="1">
-      <c r="C225" s="22"/>
+      <c r="C225" s="25"/>
     </row>
     <row r="226" ht="12.75" customHeight="1">
-      <c r="C226" s="22"/>
+      <c r="C226" s="25"/>
     </row>
     <row r="227" ht="12.75" customHeight="1">
-      <c r="C227" s="22"/>
+      <c r="C227" s="25"/>
     </row>
     <row r="228" ht="12.75" customHeight="1">
-      <c r="C228" s="22"/>
+      <c r="C228" s="25"/>
     </row>
     <row r="229" ht="12.75" customHeight="1">
-      <c r="C229" s="22"/>
+      <c r="C229" s="25"/>
     </row>
     <row r="230" ht="12.75" customHeight="1">
-      <c r="C230" s="22"/>
+      <c r="C230" s="25"/>
     </row>
     <row r="231" ht="12.75" customHeight="1">
-      <c r="C231" s="22"/>
+      <c r="C231" s="25"/>
     </row>
     <row r="232" ht="12.75" customHeight="1">
-      <c r="C232" s="22"/>
+      <c r="C232" s="25"/>
     </row>
     <row r="233" ht="12.75" customHeight="1">
-      <c r="C233" s="22"/>
+      <c r="C233" s="25"/>
     </row>
     <row r="234" ht="12.75" customHeight="1">
-      <c r="C234" s="22"/>
+      <c r="C234" s="25"/>
     </row>
     <row r="235" ht="12.75" customHeight="1">
-      <c r="C235" s="22"/>
+      <c r="C235" s="25"/>
     </row>
     <row r="236" ht="12.75" customHeight="1">
-      <c r="C236" s="22"/>
+      <c r="C236" s="25"/>
     </row>
     <row r="237" ht="12.75" customHeight="1">
-      <c r="C237" s="22"/>
+      <c r="C237" s="25"/>
     </row>
     <row r="238" ht="12.75" customHeight="1">
-      <c r="C238" s="22"/>
+      <c r="C238" s="25"/>
     </row>
     <row r="239" ht="12.75" customHeight="1">
-      <c r="C239" s="22"/>
+      <c r="C239" s="25"/>
     </row>
     <row r="240" ht="12.75" customHeight="1">
-      <c r="C240" s="22"/>
+      <c r="C240" s="25"/>
     </row>
     <row r="241" ht="12.75" customHeight="1">
-      <c r="C241" s="22"/>
+      <c r="C241" s="25"/>
     </row>
     <row r="242" ht="12.75" customHeight="1">
-      <c r="C242" s="22"/>
+      <c r="C242" s="25"/>
     </row>
     <row r="243" ht="12.75" customHeight="1">
-      <c r="C243" s="22"/>
+      <c r="C243" s="25"/>
     </row>
     <row r="244" ht="12.75" customHeight="1">
-      <c r="C244" s="22"/>
+      <c r="C244" s="25"/>
     </row>
     <row r="245" ht="12.75" customHeight="1">
-      <c r="C245" s="22"/>
+      <c r="C245" s="25"/>
     </row>
     <row r="246" ht="12.75" customHeight="1">
-      <c r="C246" s="22"/>
+      <c r="C246" s="25"/>
     </row>
     <row r="247" ht="12.75" customHeight="1">
-      <c r="C247" s="22"/>
+      <c r="C247" s="25"/>
     </row>
     <row r="248" ht="12.75" customHeight="1">
-      <c r="C248" s="22"/>
+      <c r="C248" s="25"/>
     </row>
     <row r="249" ht="12.75" customHeight="1">
-      <c r="C249" s="22"/>
+      <c r="C249" s="25"/>
     </row>
     <row r="250" ht="12.75" customHeight="1">
-      <c r="C250" s="22"/>
+      <c r="C250" s="25"/>
     </row>
     <row r="251" ht="12.75" customHeight="1">
-      <c r="C251" s="22"/>
+      <c r="C251" s="25"/>
     </row>
     <row r="252" ht="12.75" customHeight="1">
-      <c r="C252" s="22"/>
+      <c r="C252" s="25"/>
     </row>
     <row r="253" ht="12.75" customHeight="1">
-      <c r="C253" s="22"/>
+      <c r="C253" s="25"/>
     </row>
     <row r="254" ht="12.75" customHeight="1">
-      <c r="C254" s="22"/>
+      <c r="C254" s="25"/>
     </row>
     <row r="255" ht="12.75" customHeight="1">
-      <c r="C255" s="22"/>
+      <c r="C255" s="25"/>
     </row>
     <row r="256" ht="12.75" customHeight="1">
-      <c r="C256" s="22"/>
+      <c r="C256" s="25"/>
     </row>
     <row r="257" ht="12.75" customHeight="1">
-      <c r="C257" s="22"/>
+      <c r="C257" s="25"/>
     </row>
     <row r="258" ht="12.75" customHeight="1">
-      <c r="C258" s="22"/>
+      <c r="C258" s="25"/>
     </row>
     <row r="259" ht="12.75" customHeight="1">
-      <c r="C259" s="22"/>
+      <c r="C259" s="25"/>
     </row>
     <row r="260" ht="12.75" customHeight="1">
-      <c r="C260" s="22"/>
+      <c r="C260" s="25"/>
     </row>
     <row r="261" ht="12.75" customHeight="1">
-      <c r="C261" s="22"/>
+      <c r="C261" s="25"/>
     </row>
     <row r="262" ht="12.75" customHeight="1">
-      <c r="C262" s="22"/>
+      <c r="C262" s="25"/>
     </row>
     <row r="263" ht="12.75" customHeight="1">
-      <c r="C263" s="22"/>
+      <c r="C263" s="25"/>
     </row>
     <row r="264" ht="12.75" customHeight="1">
-      <c r="C264" s="22"/>
+      <c r="C264" s="25"/>
     </row>
     <row r="265" ht="12.75" customHeight="1">
-      <c r="C265" s="22"/>
+      <c r="C265" s="25"/>
     </row>
     <row r="266" ht="12.75" customHeight="1">
-      <c r="C266" s="22"/>
+      <c r="C266" s="25"/>
     </row>
     <row r="267" ht="12.75" customHeight="1">
-      <c r="C267" s="22"/>
+      <c r="C267" s="25"/>
     </row>
     <row r="268" ht="12.75" customHeight="1">
-      <c r="C268" s="22"/>
+      <c r="C268" s="25"/>
     </row>
     <row r="269" ht="12.75" customHeight="1">
-      <c r="C269" s="22"/>
+      <c r="C269" s="25"/>
     </row>
     <row r="270" ht="12.75" customHeight="1">
-      <c r="C270" s="22"/>
+      <c r="C270" s="25"/>
     </row>
     <row r="271" ht="12.75" customHeight="1">
-      <c r="C271" s="22"/>
+      <c r="C271" s="25"/>
     </row>
     <row r="272" ht="12.75" customHeight="1">
-      <c r="C272" s="22"/>
+      <c r="C272" s="25"/>
     </row>
     <row r="273" ht="12.75" customHeight="1">
-      <c r="C273" s="22"/>
+      <c r="C273" s="25"/>
     </row>
     <row r="274" ht="12.75" customHeight="1">
-      <c r="C274" s="22"/>
+      <c r="C274" s="25"/>
     </row>
     <row r="275" ht="12.75" customHeight="1">
-      <c r="C275" s="22"/>
+      <c r="C275" s="25"/>
     </row>
     <row r="276" ht="12.75" customHeight="1">
-      <c r="C276" s="22"/>
+      <c r="C276" s="25"/>
     </row>
     <row r="277" ht="12.75" customHeight="1">
-      <c r="C277" s="22"/>
+      <c r="C277" s="25"/>
     </row>
     <row r="278" ht="12.75" customHeight="1">
-      <c r="C278" s="22"/>
+      <c r="C278" s="25"/>
     </row>
     <row r="279" ht="12.75" customHeight="1">
-      <c r="C279" s="22"/>
+      <c r="C279" s="25"/>
     </row>
     <row r="280" ht="12.75" customHeight="1">
-      <c r="C280" s="22"/>
+      <c r="C280" s="25"/>
     </row>
     <row r="281" ht="12.75" customHeight="1">
-      <c r="C281" s="22"/>
+      <c r="C281" s="25"/>
     </row>
     <row r="282" ht="12.75" customHeight="1">
-      <c r="C282" s="22"/>
+      <c r="C282" s="25"/>
     </row>
     <row r="283" ht="12.75" customHeight="1">
-      <c r="C283" s="22"/>
+      <c r="C283" s="25"/>
     </row>
     <row r="284" ht="12.75" customHeight="1">
-      <c r="C284" s="22"/>
+      <c r="C284" s="25"/>
     </row>
     <row r="285" ht="12.75" customHeight="1">
-      <c r="C285" s="22"/>
+      <c r="C285" s="25"/>
     </row>
     <row r="286" ht="12.75" customHeight="1">
-      <c r="C286" s="22"/>
+      <c r="C286" s="25"/>
     </row>
     <row r="287" ht="12.75" customHeight="1">
-      <c r="C287" s="22"/>
+      <c r="C287" s="25"/>
     </row>
     <row r="288" ht="12.75" customHeight="1">
-      <c r="C288" s="22"/>
+      <c r="C288" s="25"/>
     </row>
     <row r="289" ht="12.75" customHeight="1">
-      <c r="C289" s="22"/>
+      <c r="C289" s="25"/>
     </row>
     <row r="290" ht="12.75" customHeight="1">
-      <c r="C290" s="22"/>
+      <c r="C290" s="25"/>
     </row>
     <row r="291" ht="12.75" customHeight="1">
-      <c r="C291" s="22"/>
+      <c r="C291" s="25"/>
     </row>
     <row r="292" ht="15.75" customHeight="1"/>
     <row r="293" ht="15.75" customHeight="1"/>

</xml_diff>